<commit_message>
Apply frozen header to all modified templates.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Experiment_run_MGI_v4_4_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Experiment_run_MGI_v4_4_0.xlsx
@@ -185,6 +185,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Sample </t>
     </r>
@@ -1565,7 +1566,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1637,6 +1638,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1648,13 +1650,6 @@
     </font>
     <font>
       <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1778,7 +1773,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1859,19 +1854,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1879,15 +1874,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1971,7 +1962,9 @@
   <dimension ref="A1:R1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10121,7 +10114,9 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17519,7 +17514,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.38"/>
   </cols>
@@ -17697,7 +17692,7 @@
       <c r="A25" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="23" t="s">
         <v>55</v>
       </c>
       <c r="C25" s="24"/>
@@ -17721,16 +17716,16 @@
       <c r="C27" s="24"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">

</xml_diff>